<commit_message>
Completed the validation of the functional model with accurate interfaces and corrected a bug in the use of the quantum keeper
</commit_message>
<xml_diff>
--- a/processors/LEON2/LEON2_func_ValidationResults.xlsx
+++ b/processors/LEON2/LEON2_func_ValidationResults.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="4" r:id="rId1"/>
     <sheet name="TSIM" sheetId="1" r:id="rId2"/>
     <sheet name="TSIM-HW" sheetId="2" r:id="rId3"/>
-    <sheet name="GRSIM" sheetId="5" r:id="rId4"/>
-    <sheet name="Foglio1" sheetId="6" r:id="rId5"/>
+    <sheet name="GRSIM LT" sheetId="5" r:id="rId4"/>
+    <sheet name="GRSIM AT" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">GRSIM!$A$4:$O$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'GRSIM AT'!$A$4:$O$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'GRSIM LT'!$A$4:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TSIM!$A$4:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TSIM-HW'!$A$4:$O$4</definedName>
   </definedNames>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="97">
   <si>
     <t>total_cycles</t>
   </si>
@@ -882,7 +883,302 @@
     <cellStyle name="Valore non valido" xfId="2" builtinId="27"/>
     <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="116">
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="3" tint="-0.499984740745262"/>
@@ -5553,127 +5849,127 @@
     <mergeCell ref="K2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:J60">
-    <cfRule type="cellIs" dxfId="83" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="25" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C60">
-    <cfRule type="cellIs" dxfId="82" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="24" operator="greaterThan">
       <formula>D5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:L2">
-    <cfRule type="cellIs" dxfId="81" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="23" operator="greaterThan">
       <formula>L2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:F60">
-    <cfRule type="expression" dxfId="80" priority="22">
+    <cfRule type="expression" dxfId="112" priority="22">
       <formula>$E5-$F5 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:J83">
-    <cfRule type="cellIs" dxfId="79" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="78" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="20" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82:G82">
-    <cfRule type="expression" dxfId="77" priority="19">
+    <cfRule type="expression" dxfId="109" priority="19">
       <formula>$E82-$F82 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84">
-    <cfRule type="cellIs" dxfId="76" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="75" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="17" operator="greaterThan">
       <formula>D84</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85">
-    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="16" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="cellIs" dxfId="73" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="15" operator="greaterThan">
       <formula>D85</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:H85 H86">
-    <cfRule type="expression" dxfId="72" priority="14">
+    <cfRule type="expression" dxfId="104" priority="14">
       <formula>$E85-$F85 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86">
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="13" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="70" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="12" operator="greaterThan">
       <formula>D86</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:G86">
-    <cfRule type="expression" dxfId="69" priority="11">
+    <cfRule type="expression" dxfId="101" priority="11">
       <formula>$E86-$F86 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="68" priority="10">
+    <cfRule type="expression" dxfId="100" priority="10">
       <formula>$E87-$F87 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87">
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="9" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="66" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="8" operator="greaterThan">
       <formula>D87</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87:G87">
-    <cfRule type="expression" dxfId="65" priority="7">
+    <cfRule type="expression" dxfId="97" priority="7">
       <formula>$E87-$F87 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="64" priority="6">
+    <cfRule type="expression" dxfId="96" priority="6">
       <formula>$E87-$F87 &lt;&gt; -1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="5" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="62" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="4" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="61" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="3" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="60" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="2" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="1" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9451,137 +9747,137 @@
     <mergeCell ref="C63:K80"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:J60 J82:J89">
-    <cfRule type="cellIs" dxfId="58" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="41" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C60">
-    <cfRule type="cellIs" dxfId="57" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="40" operator="greaterThan">
       <formula>D5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="56" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="39" operator="greaterThan">
       <formula>L2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:F60">
-    <cfRule type="expression" dxfId="55" priority="38">
+    <cfRule type="expression" dxfId="87" priority="38">
       <formula>((ABS($E5-$F5))/$E5) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="54" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="36" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82:F82">
-    <cfRule type="expression" dxfId="53" priority="35">
+    <cfRule type="expression" dxfId="85" priority="35">
       <formula>((ABS($E82-$F82))/$E82) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="52" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="33" operator="greaterThan">
       <formula>D83</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83:F83">
-    <cfRule type="expression" dxfId="51" priority="32">
+    <cfRule type="expression" dxfId="83" priority="32">
       <formula>((ABS($E83-$F83))/$E83) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="50" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="30" operator="greaterThan">
       <formula>D84</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:F84">
-    <cfRule type="expression" dxfId="49" priority="29">
+    <cfRule type="expression" dxfId="81" priority="29">
       <formula>((ABS($E84-$F84))/$E84) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" dxfId="48" priority="28">
+    <cfRule type="expression" dxfId="80" priority="28">
       <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="cellIs" dxfId="47" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="26" operator="greaterThan">
       <formula>D85</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:F85">
-    <cfRule type="expression" dxfId="46" priority="25">
+    <cfRule type="expression" dxfId="78" priority="25">
       <formula>((ABS($E85-$F85))/$E85) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="45" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="23" operator="greaterThan">
       <formula>D86</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:F86">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="76" priority="22">
       <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" dxfId="43" priority="21">
+    <cfRule type="expression" dxfId="75" priority="21">
       <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="42" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="19" operator="greaterThan">
       <formula>D87</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87:F87">
-    <cfRule type="expression" dxfId="41" priority="18">
+    <cfRule type="expression" dxfId="73" priority="18">
       <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="17" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="cellIs" dxfId="39" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="16" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="38" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="52" operator="greaterThan">
       <formula>D88</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="cellIs" dxfId="37" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="55" operator="greaterThan">
       <formula>D89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="5" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="3" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="2" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9594,9 +9890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82:A91"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13337,162 +13633,162 @@
     <mergeCell ref="C63:K80"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:J60 J82:J91">
-    <cfRule type="cellIs" dxfId="31" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="46" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C60">
-    <cfRule type="cellIs" dxfId="30" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="45" operator="greaterThan">
       <formula>D5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="29" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="44" operator="greaterThan">
       <formula>L2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:F60">
-    <cfRule type="expression" dxfId="28" priority="43">
+    <cfRule type="expression" dxfId="60" priority="43">
       <formula>((ABS($E5-$F5))/$E5) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C88">
-    <cfRule type="cellIs" dxfId="27" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="41" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82:F82">
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="58" priority="40">
       <formula>((ABS($E82-$F82))/$E82) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="25" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="38" operator="greaterThan">
       <formula>D83</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83:F83">
-    <cfRule type="expression" dxfId="24" priority="37">
+    <cfRule type="expression" dxfId="56" priority="37">
       <formula>((ABS($E83-$F83))/$E83) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="35" operator="greaterThan">
       <formula>D84</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:F84">
-    <cfRule type="expression" dxfId="22" priority="34">
+    <cfRule type="expression" dxfId="54" priority="34">
       <formula>((ABS($E84-$F84))/$E84) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" dxfId="21" priority="33">
+    <cfRule type="expression" dxfId="53" priority="33">
       <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="31" operator="greaterThan">
       <formula>D85</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:F85">
-    <cfRule type="expression" dxfId="19" priority="30">
+    <cfRule type="expression" dxfId="51" priority="30">
       <formula>((ABS($E85-$F85))/$E85) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="28" operator="greaterThan">
       <formula>D86</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:F86">
-    <cfRule type="expression" dxfId="17" priority="27">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" dxfId="16" priority="26">
+    <cfRule type="expression" dxfId="48" priority="26">
       <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87:C88">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="greaterThan">
       <formula>D87</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87:F87">
-    <cfRule type="expression" dxfId="14" priority="23">
+    <cfRule type="expression" dxfId="46" priority="23">
       <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C88">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C88">
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="21" operator="greaterThan">
       <formula>D82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="greaterThan">
       <formula>D89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="greaterThan">
       <formula>D89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="greaterThan">
       <formula>D89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="greaterThan">
       <formula>D89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="13" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="greaterThan">
       <formula>D90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="greaterThan">
       <formula>D91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThan">
       <formula>D91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
       <formula>D91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThan">
       <formula>D91</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13503,12 +13799,3911 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="67" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="C1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="16"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="C2" s="14">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <f>AVERAGE($J$5:$J$60)</f>
+        <v>6.6862991103980507E-3</v>
+      </c>
+      <c r="H2" s="5">
+        <f>STDEV($J$5:$J$60)</f>
+        <v>1.277975681281293E-2</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="27"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="3" t="str">
+        <f>TSIM!A5</f>
+        <v>AES.O0</v>
+      </c>
+      <c r="B5">
+        <v>275147353</v>
+      </c>
+      <c r="C5" s="5">
+        <f>B5-($C$2*F5+G5*$D$2+H5*$E$2)</f>
+        <v>56646081</v>
+      </c>
+      <c r="D5">
+        <v>56646085</v>
+      </c>
+      <c r="E5">
+        <v>52994060</v>
+      </c>
+      <c r="F5">
+        <f>TSIM!F5</f>
+        <v>52994061</v>
+      </c>
+      <c r="G5">
+        <f>TSIM!G5</f>
+        <v>5873001</v>
+      </c>
+      <c r="H5">
+        <f>TSIM!H5</f>
+        <v>652027</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" ref="J5:J60" si="0">IF(D5 = 0, "", ABS(C5-D5)/D5)</f>
+        <v>7.0613882671679784E-8</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" ref="K5:K60" si="1">B5/E5</f>
+        <v>5.1920413910540164</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L60" si="2">B5-D5</f>
+        <v>218501268</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" ref="M5:M60" si="3">L5/E5</f>
+        <v>4.1231275354256685</v>
+      </c>
+      <c r="N5">
+        <f>E5-F5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="3" t="str">
+        <f>TSIM!A6</f>
+        <v>AES.O1</v>
+      </c>
+      <c r="B6">
+        <v>172390580</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C60" si="4">B6-($C$2*F6+G6*$D$2+H6*$E$2)</f>
+        <v>36266127</v>
+      </c>
+      <c r="D6">
+        <v>36266130</v>
+      </c>
+      <c r="E6">
+        <v>32706106</v>
+      </c>
+      <c r="F6">
+        <f>TSIM!F6</f>
+        <v>32706107</v>
+      </c>
+      <c r="G6">
+        <f>TSIM!G6</f>
+        <v>4740000</v>
+      </c>
+      <c r="H6">
+        <f>TSIM!H6</f>
+        <v>560025</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2721812335642097E-8</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2708989569103704</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="2"/>
+        <v>136124450</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1620500465570558</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N60" si="5">E6-F6</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="3" t="str">
+        <f>TSIM!A7</f>
+        <v>AES.O2</v>
+      </c>
+      <c r="B7">
+        <v>172280575</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="4"/>
+        <v>36244126</v>
+      </c>
+      <c r="D7">
+        <v>36244129</v>
+      </c>
+      <c r="E7">
+        <v>32684105</v>
+      </c>
+      <c r="F7">
+        <f>TSIM!F7</f>
+        <v>32684106</v>
+      </c>
+      <c r="G7">
+        <f>TSIM!G7</f>
+        <v>4740000</v>
+      </c>
+      <c r="H7">
+        <f>TSIM!H7</f>
+        <v>560025</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2772026332871729E-8</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2710813100129252</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="2"/>
+        <v>136036446</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1621591290322923</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="3" t="str">
+        <f>TSIM!A8</f>
+        <v>AES.O3</v>
+      </c>
+      <c r="B8">
+        <v>170325570</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="4"/>
+        <v>35873125</v>
+      </c>
+      <c r="D8">
+        <v>35873128</v>
+      </c>
+      <c r="E8">
+        <v>32313104</v>
+      </c>
+      <c r="F8">
+        <f>TSIM!F8</f>
+        <v>32313105</v>
+      </c>
+      <c r="G8">
+        <f>TSIM!G8</f>
+        <v>4640000</v>
+      </c>
+      <c r="H8">
+        <f>TSIM!H8</f>
+        <v>560025</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3628057190886731E-8</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2710989943893969</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="2"/>
+        <v>134452442</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1609262298044785</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="3" t="str">
+        <f>TSIM!A9</f>
+        <v>bcnt.O0</v>
+      </c>
+      <c r="B9">
+        <v>90990122</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="4"/>
+        <v>18305021</v>
+      </c>
+      <c r="D9">
+        <v>18305025</v>
+      </c>
+      <c r="E9">
+        <v>16200023</v>
+      </c>
+      <c r="F9">
+        <f>TSIM!F9</f>
+        <v>16200024</v>
+      </c>
+      <c r="G9">
+        <f>TSIM!G9</f>
+        <v>5780001</v>
+      </c>
+      <c r="H9">
+        <f>TSIM!H9</f>
+        <v>2105004</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1851923174101101E-7</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="1"/>
+        <v>5.6166662232516584</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="2"/>
+        <v>72685097</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="3"/>
+        <v>4.4867280126701052</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="3" t="str">
+        <f>TSIM!A10</f>
+        <v>bcnt.O1</v>
+      </c>
+      <c r="B10" s="4">
+        <v>66600132</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="4"/>
+        <v>13505022</v>
+      </c>
+      <c r="D10">
+        <v>13500026</v>
+      </c>
+      <c r="E10" s="4">
+        <v>11570026</v>
+      </c>
+      <c r="F10">
+        <f>TSIM!F10</f>
+        <v>11570027</v>
+      </c>
+      <c r="G10">
+        <f>TSIM!G10</f>
+        <v>4885000</v>
+      </c>
+      <c r="H10">
+        <f>TSIM!H10</f>
+        <v>1930002</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7007336134019296E-4</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="1"/>
+        <v>5.7562646790940661</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="2"/>
+        <v>53100106</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="3"/>
+        <v>4.589454336576253</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="3" t="str">
+        <f>TSIM!A11</f>
+        <v>bcnt.O2</v>
+      </c>
+      <c r="B11" s="4">
+        <v>66600132</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="4"/>
+        <v>13505022</v>
+      </c>
+      <c r="D11" s="9">
+        <v>13500026</v>
+      </c>
+      <c r="E11" s="4">
+        <v>11570026</v>
+      </c>
+      <c r="F11" s="9">
+        <f>TSIM!F11</f>
+        <v>11570027</v>
+      </c>
+      <c r="G11" s="9">
+        <f>TSIM!G11</f>
+        <v>4885000</v>
+      </c>
+      <c r="H11" s="9">
+        <f>TSIM!H11</f>
+        <v>1930002</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7007336134019296E-4</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="1"/>
+        <v>5.7562646790940661</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="2"/>
+        <v>53100106</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="3"/>
+        <v>4.589454336576253</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="3" t="str">
+        <f>TSIM!A12</f>
+        <v>bcnt.O3</v>
+      </c>
+      <c r="B12" s="4">
+        <v>66600132</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="4"/>
+        <v>13505022</v>
+      </c>
+      <c r="D12" s="9">
+        <v>13500026</v>
+      </c>
+      <c r="E12" s="4">
+        <v>11570026</v>
+      </c>
+      <c r="F12" s="9">
+        <f>TSIM!F12</f>
+        <v>11570027</v>
+      </c>
+      <c r="G12" s="9">
+        <f>TSIM!G12</f>
+        <v>4885000</v>
+      </c>
+      <c r="H12" s="9">
+        <f>TSIM!H12</f>
+        <v>1930002</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7007336134019296E-4</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="1"/>
+        <v>5.7562646790940661</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="2"/>
+        <v>53100106</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="3"/>
+        <v>4.589454336576253</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3" t="str">
+        <f>TSIM!A13</f>
+        <v>blit.O0</v>
+      </c>
+      <c r="B13" s="4">
+        <v>319397144</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="4"/>
+        <v>66290233</v>
+      </c>
+      <c r="D13">
+        <v>66290237</v>
+      </c>
+      <c r="E13" s="4">
+        <v>54246205</v>
+      </c>
+      <c r="F13">
+        <f>TSIM!F13</f>
+        <v>54246206</v>
+      </c>
+      <c r="G13">
+        <f>TSIM!G13</f>
+        <v>24080055</v>
+      </c>
+      <c r="H13">
+        <f>TSIM!H13</f>
+        <v>12042032</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13" s="6">
+        <f t="shared" si="0"/>
+        <v>6.034071050311677E-8</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="1"/>
+        <v>5.887916841371668</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="2"/>
+        <v>253106907</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6658915033779786</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="3" t="str">
+        <f>TSIM!A14</f>
+        <v>blit.O1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>96673632</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="4"/>
+        <v>20137123</v>
+      </c>
+      <c r="D14">
+        <v>20137127</v>
+      </c>
+      <c r="E14" s="4">
+        <v>18131124</v>
+      </c>
+      <c r="F14">
+        <f>TSIM!F14</f>
+        <v>18131125</v>
+      </c>
+      <c r="G14">
+        <f>TSIM!G14</f>
+        <v>2008006</v>
+      </c>
+      <c r="H14">
+        <f>TSIM!H14</f>
+        <v>2004003</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9863806788326855E-7</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3319161018368195</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="2"/>
+        <v>76536505</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2212774563783251</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="3" t="str">
+        <f>TSIM!A15</f>
+        <v>blit.O2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>96648602</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="4"/>
+        <v>20132117</v>
+      </c>
+      <c r="D15">
+        <v>20132121</v>
+      </c>
+      <c r="E15" s="4">
+        <v>18126118</v>
+      </c>
+      <c r="F15">
+        <f>TSIM!F15</f>
+        <v>18126119</v>
+      </c>
+      <c r="G15">
+        <f>TSIM!G15</f>
+        <v>2008006</v>
+      </c>
+      <c r="H15">
+        <f>TSIM!H15</f>
+        <v>2004003</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9868746070024117E-7</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3320077691207795</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="2"/>
+        <v>76516481</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="3"/>
+        <v>4.221338567916197</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="3" t="str">
+        <f>TSIM!A16</f>
+        <v>blit.O3</v>
+      </c>
+      <c r="B16" s="4">
+        <v>96648602</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="4"/>
+        <v>20132117</v>
+      </c>
+      <c r="D16" s="9">
+        <v>20132121</v>
+      </c>
+      <c r="E16" s="4">
+        <v>18126118</v>
+      </c>
+      <c r="F16" s="9">
+        <f>TSIM!F16</f>
+        <v>18126119</v>
+      </c>
+      <c r="G16" s="9">
+        <f>TSIM!G16</f>
+        <v>2008006</v>
+      </c>
+      <c r="H16" s="9">
+        <f>TSIM!H16</f>
+        <v>2004003</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9868746070024117E-7</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3320077691207795</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="2"/>
+        <v>76516481</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="3"/>
+        <v>4.221338567916197</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="3" t="str">
+        <f>TSIM!A17</f>
+        <v>crc.O0</v>
+      </c>
+      <c r="B17" s="18">
+        <v>185953762</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="4"/>
+        <v>36956592</v>
+      </c>
+      <c r="D17">
+        <v>36956596</v>
+      </c>
+      <c r="E17" s="18">
+        <v>34269426</v>
+      </c>
+      <c r="F17">
+        <f>TSIM!F17</f>
+        <v>34269427</v>
+      </c>
+      <c r="G17">
+        <f>TSIM!G17</f>
+        <v>9252546</v>
+      </c>
+      <c r="H17">
+        <f>TSIM!H17</f>
+        <v>2666916</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0823507662881072E-7</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4262292575311886</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="2"/>
+        <v>148997166</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3478162137877652</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="3" t="str">
+        <f>TSIM!A18</f>
+        <v>crc.O1</v>
+      </c>
+      <c r="B18" s="18">
+        <v>79093289</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="4"/>
+        <v>15503063</v>
+      </c>
+      <c r="D18">
+        <v>15503067</v>
+      </c>
+      <c r="E18" s="18">
+        <v>15482299</v>
+      </c>
+      <c r="F18">
+        <f>TSIM!F18</f>
+        <v>15482300</v>
+      </c>
+      <c r="G18">
+        <f>TSIM!G18</f>
+        <v>1660512</v>
+      </c>
+      <c r="H18">
+        <f>TSIM!H18</f>
+        <v>514</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5801346275546639E-7</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1086268906187637</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="2"/>
+        <v>63590222</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1072854877689675</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="3" t="str">
+        <f>TSIM!A19</f>
+        <v>crc.O2</v>
+      </c>
+      <c r="B19" s="18">
+        <v>75091999</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="4"/>
+        <v>14702805</v>
+      </c>
+      <c r="D19">
+        <v>14702809</v>
+      </c>
+      <c r="E19" s="18">
+        <v>14682041</v>
+      </c>
+      <c r="F19">
+        <f>TSIM!F19</f>
+        <v>14682042</v>
+      </c>
+      <c r="G19">
+        <f>TSIM!G19</f>
+        <v>1660512</v>
+      </c>
+      <c r="H19">
+        <f>TSIM!H19</f>
+        <v>514</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7205685661835093E-7</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1145476981027365</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="2"/>
+        <v>60389190</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1131331808704257</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="3" t="str">
+        <f>TSIM!A20</f>
+        <v>crc.O3</v>
+      </c>
+      <c r="B20" s="18">
+        <v>62700959</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="4"/>
+        <v>12224597</v>
+      </c>
+      <c r="D20">
+        <v>12224601</v>
+      </c>
+      <c r="E20" s="18">
+        <v>12203833</v>
+      </c>
+      <c r="F20">
+        <f>TSIM!F20</f>
+        <v>12203834</v>
+      </c>
+      <c r="G20">
+        <f>TSIM!G20</f>
+        <v>1660512</v>
+      </c>
+      <c r="H20">
+        <f>TSIM!H20</f>
+        <v>514</v>
+      </c>
+      <c r="I20"/>
+      <c r="J20" s="6">
+        <f t="shared" si="0"/>
+        <v>3.272090434689852E-7</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1378086704398527</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="2"/>
+        <v>50476358</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1361069100175332</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="3" t="str">
+        <f>TSIM!A21</f>
+        <v>des.O0</v>
+      </c>
+      <c r="B21" s="18">
+        <v>31676451</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="4"/>
+        <v>6298707</v>
+      </c>
+      <c r="D21">
+        <v>6298711</v>
+      </c>
+      <c r="E21" s="18">
+        <v>6194566</v>
+      </c>
+      <c r="F21">
+        <f>TSIM!F21</f>
+        <v>6194567</v>
+      </c>
+      <c r="G21">
+        <f>TSIM!G21</f>
+        <v>496433</v>
+      </c>
+      <c r="H21">
+        <f>TSIM!H21</f>
+        <v>103043</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="0"/>
+        <v>6.3505056828293919E-7</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1135868114085801</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="2"/>
+        <v>25377740</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="3"/>
+        <v>4.0967744955820953</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="3" t="str">
+        <f>TSIM!A22</f>
+        <v>des.O1</v>
+      </c>
+      <c r="B22" s="18">
+        <v>23745653</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="4"/>
+        <v>4711148</v>
+      </c>
+      <c r="D22">
+        <v>4711152</v>
+      </c>
+      <c r="E22" s="18">
+        <v>4611425</v>
+      </c>
+      <c r="F22">
+        <f>TSIM!F22</f>
+        <v>4611426</v>
+      </c>
+      <c r="G22">
+        <f>TSIM!G22</f>
+        <v>490176</v>
+      </c>
+      <c r="H22">
+        <f>TSIM!H22</f>
+        <v>98625</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4904923466701983E-7</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1493091614847906</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="2"/>
+        <v>19034501</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1276830914522087</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="3" t="str">
+        <f>TSIM!A23</f>
+        <v>des.O2</v>
+      </c>
+      <c r="B23" s="18">
+        <v>23824773</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="4"/>
+        <v>4726972</v>
+      </c>
+      <c r="D23">
+        <v>4726976</v>
+      </c>
+      <c r="E23" s="18">
+        <v>4627249</v>
+      </c>
+      <c r="F23">
+        <f>TSIM!F23</f>
+        <v>4627250</v>
+      </c>
+      <c r="G23">
+        <f>TSIM!G23</f>
+        <v>490176</v>
+      </c>
+      <c r="H23">
+        <f>TSIM!H23</f>
+        <v>98625</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="0"/>
+        <v>8.462069619139171E-7</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1487985626016668</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="2"/>
+        <v>19097797</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1272464481595872</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="3" t="str">
+        <f>TSIM!A24</f>
+        <v>des.O3</v>
+      </c>
+      <c r="B24" s="18">
+        <v>23778773</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="4"/>
+        <v>4717772</v>
+      </c>
+      <c r="D24">
+        <v>4717776</v>
+      </c>
+      <c r="E24" s="18">
+        <v>4618049</v>
+      </c>
+      <c r="F24">
+        <f>TSIM!F24</f>
+        <v>4618050</v>
+      </c>
+      <c r="G24">
+        <f>TSIM!G24</f>
+        <v>490176</v>
+      </c>
+      <c r="H24">
+        <f>TSIM!H24</f>
+        <v>98625</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4785712590000032E-7</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1490949966100406</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="2"/>
+        <v>19060997</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1274999464059388</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="3" t="str">
+        <f>TSIM!A25</f>
+        <v>engine.O0</v>
+      </c>
+      <c r="B25" s="18">
+        <v>280983196</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="4"/>
+        <v>69975887</v>
+      </c>
+      <c r="D25">
+        <v>69975891</v>
+      </c>
+      <c r="E25" s="18">
+        <v>48838226</v>
+      </c>
+      <c r="F25">
+        <f>TSIM!F25</f>
+        <v>48838227</v>
+      </c>
+      <c r="G25">
+        <f>TSIM!G25</f>
+        <v>11476070</v>
+      </c>
+      <c r="H25">
+        <f>TSIM!H25</f>
+        <v>4178331</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="0"/>
+        <v>5.7162544739873334E-8</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="1"/>
+        <v>5.7533456682067037</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="2"/>
+        <v>211007305</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3205358237213609</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="3" t="str">
+        <f>TSIM!A26</f>
+        <v>engine.O1</v>
+      </c>
+      <c r="B26" s="18">
+        <v>135224796</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="4"/>
+        <v>41503444</v>
+      </c>
+      <c r="D26">
+        <v>41258444</v>
+      </c>
+      <c r="E26" s="18">
+        <v>21937503</v>
+      </c>
+      <c r="F26">
+        <f>TSIM!F26</f>
+        <v>21937504</v>
+      </c>
+      <c r="G26">
+        <f>TSIM!G26</f>
+        <v>3609729</v>
+      </c>
+      <c r="H26">
+        <f>TSIM!H26</f>
+        <v>2361607</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="0"/>
+        <v>5.9381783762858338E-3</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="1"/>
+        <v>6.1640924220044555</v>
+      </c>
+      <c r="L26" s="4">
+        <f t="shared" si="2"/>
+        <v>93966352</v>
+      </c>
+      <c r="M26" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2833658871750355</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="3" t="str">
+        <f>TSIM!A27</f>
+        <v>engine.O2</v>
+      </c>
+      <c r="B27" s="18">
+        <v>115230807</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="4"/>
+        <v>37522588</v>
+      </c>
+      <c r="D27">
+        <v>37190633</v>
+      </c>
+      <c r="E27" s="18">
+        <v>18222255</v>
+      </c>
+      <c r="F27">
+        <f>TSIM!F27</f>
+        <v>18222256</v>
+      </c>
+      <c r="G27">
+        <f>TSIM!G27</f>
+        <v>2810151</v>
+      </c>
+      <c r="H27">
+        <f>TSIM!H27</f>
+        <v>2009044</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="0"/>
+        <v>8.9257690236140916E-3</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="1"/>
+        <v>6.3236304727378689</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="2"/>
+        <v>78040174</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2826847719999526</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="3" t="str">
+        <f>TSIM!A28</f>
+        <v>engine.O3</v>
+      </c>
+      <c r="B28" s="18">
+        <v>115391457</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="4"/>
+        <v>37567978</v>
+      </c>
+      <c r="D28">
+        <v>37219448</v>
+      </c>
+      <c r="E28" s="18">
+        <v>18251070</v>
+      </c>
+      <c r="F28">
+        <f>TSIM!F28</f>
+        <v>18251071</v>
+      </c>
+      <c r="G28">
+        <f>TSIM!G28</f>
+        <v>2810151</v>
+      </c>
+      <c r="H28">
+        <f>TSIM!H28</f>
+        <v>2009044</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3641904630074047E-3</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="1"/>
+        <v>6.3224488756001707</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="2"/>
+        <v>78172009</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2831466319508937</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="3" t="str">
+        <f>TSIM!A29</f>
+        <v>fib.O0</v>
+      </c>
+      <c r="B29" s="18">
+        <v>185246797</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="4"/>
+        <v>41684438</v>
+      </c>
+      <c r="D29">
+        <v>39883842</v>
+      </c>
+      <c r="E29" s="18">
+        <v>34304914</v>
+      </c>
+      <c r="F29">
+        <f>TSIM!F29</f>
+        <v>34304915</v>
+      </c>
+      <c r="G29">
+        <f>TSIM!G29</f>
+        <v>4078409</v>
+      </c>
+      <c r="H29">
+        <f>TSIM!H29</f>
+        <v>2264290</v>
+      </c>
+      <c r="I29"/>
+      <c r="K29" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4000076198995863</v>
+      </c>
+      <c r="L29" s="4">
+        <f t="shared" si="2"/>
+        <v>145362955</v>
+      </c>
+      <c r="M29" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2373799567024131</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O29" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="3" t="str">
+        <f>TSIM!A30</f>
+        <v>fib.O1</v>
+      </c>
+      <c r="B30" s="18">
+        <v>112027299</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="4"/>
+        <v>26707722</v>
+      </c>
+      <c r="D30">
+        <v>24907126</v>
+      </c>
+      <c r="E30" s="18">
+        <v>20992278</v>
+      </c>
+      <c r="F30">
+        <f>TSIM!F30</f>
+        <v>20992279</v>
+      </c>
+      <c r="G30">
+        <f>TSIM!G30</f>
+        <v>750251</v>
+      </c>
+      <c r="H30">
+        <f>TSIM!H30</f>
+        <v>600210</v>
+      </c>
+      <c r="I30"/>
+      <c r="K30" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3365956281638418</v>
+      </c>
+      <c r="L30" s="4">
+        <f t="shared" si="2"/>
+        <v>87120173</v>
+      </c>
+      <c r="M30" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1501057198270717</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O30" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="8" t="str">
+        <f>TSIM!A31</f>
+        <v>fib.O2</v>
+      </c>
+      <c r="B31" s="9">
+        <v>78431773</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="4"/>
+        <v>18188208</v>
+      </c>
+      <c r="D31" s="9">
+        <v>17075356</v>
+      </c>
+      <c r="E31" s="9">
+        <v>14852227</v>
+      </c>
+      <c r="F31" s="9">
+        <f>TSIM!F31</f>
+        <v>14852228</v>
+      </c>
+      <c r="G31" s="9">
+        <f>TSIM!G31</f>
+        <v>463691</v>
+      </c>
+      <c r="H31" s="9">
+        <f>TSIM!H31</f>
+        <v>370962</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="K31" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2808089318861073</v>
+      </c>
+      <c r="L31" s="4">
+        <f t="shared" si="2"/>
+        <v>61356417</v>
+      </c>
+      <c r="M31" s="4">
+        <f t="shared" si="3"/>
+        <v>4.13112572276198</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O31" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="8" t="str">
+        <f>TSIM!A32</f>
+        <v>fib.O3</v>
+      </c>
+      <c r="B32" s="9">
+        <v>78431773</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" si="4"/>
+        <v>18188208</v>
+      </c>
+      <c r="D32" s="9">
+        <v>17075356</v>
+      </c>
+      <c r="E32" s="9">
+        <v>14852227</v>
+      </c>
+      <c r="F32" s="9">
+        <f>TSIM!F32</f>
+        <v>14852228</v>
+      </c>
+      <c r="G32" s="9">
+        <f>TSIM!G32</f>
+        <v>463691</v>
+      </c>
+      <c r="H32" s="9">
+        <f>TSIM!H32</f>
+        <v>370962</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="K32" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2808089318861073</v>
+      </c>
+      <c r="L32" s="4">
+        <f t="shared" si="2"/>
+        <v>61356417</v>
+      </c>
+      <c r="M32" s="4">
+        <f t="shared" si="3"/>
+        <v>4.13112572276198</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="3" t="str">
+        <f>TSIM!A33</f>
+        <v>fir2.O0</v>
+      </c>
+      <c r="B33" s="18">
+        <v>191996919</v>
+      </c>
+      <c r="C33" s="5">
+        <f t="shared" si="4"/>
+        <v>41796252</v>
+      </c>
+      <c r="D33">
+        <v>41796256</v>
+      </c>
+      <c r="E33" s="18">
+        <v>34207329</v>
+      </c>
+      <c r="F33">
+        <f>TSIM!F33</f>
+        <v>34207330</v>
+      </c>
+      <c r="G33">
+        <f>TSIM!G33</f>
+        <v>11943783</v>
+      </c>
+      <c r="H33">
+        <f>TSIM!H33</f>
+        <v>1427564</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="0"/>
+        <v>9.5702351904438522E-8</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="1"/>
+        <v>5.6127421991936286</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="2"/>
+        <v>150200663</v>
+      </c>
+      <c r="M33" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3908912911616103</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="3" t="str">
+        <f>TSIM!A34</f>
+        <v>fir2.O1</v>
+      </c>
+      <c r="B34" s="18">
+        <v>53543650</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" si="4"/>
+        <v>14855065</v>
+      </c>
+      <c r="D34">
+        <v>14855069</v>
+      </c>
+      <c r="E34" s="18">
+        <v>8629545</v>
+      </c>
+      <c r="F34">
+        <f>TSIM!F34</f>
+        <v>8629546</v>
+      </c>
+      <c r="G34">
+        <f>TSIM!G34</f>
+        <v>4106240</v>
+      </c>
+      <c r="H34">
+        <f>TSIM!H34</f>
+        <v>64161</v>
+      </c>
+      <c r="I34"/>
+      <c r="J34" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6926835546842631E-7</v>
+      </c>
+      <c r="K34" s="4">
+        <f t="shared" si="1"/>
+        <v>6.2046898185246153</v>
+      </c>
+      <c r="L34" s="4">
+        <f t="shared" si="2"/>
+        <v>38688581</v>
+      </c>
+      <c r="M34" s="4">
+        <f t="shared" si="3"/>
+        <v>4.4832700912968182</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="3" t="str">
+        <f>TSIM!A35</f>
+        <v>fir2.O2</v>
+      </c>
+      <c r="B35" s="18">
+        <v>77828175</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" si="4"/>
+        <v>19612923</v>
+      </c>
+      <c r="D35">
+        <v>19612927</v>
+      </c>
+      <c r="E35" s="18">
+        <v>12547308</v>
+      </c>
+      <c r="F35">
+        <f>TSIM!F35</f>
+        <v>12547309</v>
+      </c>
+      <c r="G35">
+        <f>TSIM!G35</f>
+        <v>7121760</v>
+      </c>
+      <c r="H35">
+        <f>TSIM!H35</f>
+        <v>904256</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0394712120225604E-7</v>
+      </c>
+      <c r="K35" s="4">
+        <f t="shared" si="1"/>
+        <v>6.2027787155619354</v>
+      </c>
+      <c r="L35" s="4">
+        <f t="shared" si="2"/>
+        <v>58215248</v>
+      </c>
+      <c r="M35" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6396603956800933</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="3" t="str">
+        <f>TSIM!A36</f>
+        <v>fir2.O3</v>
+      </c>
+      <c r="B36" s="18">
+        <v>77828095</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" si="4"/>
+        <v>19612907</v>
+      </c>
+      <c r="D36">
+        <v>19612911</v>
+      </c>
+      <c r="E36" s="18">
+        <v>12547292</v>
+      </c>
+      <c r="F36">
+        <f>TSIM!F36</f>
+        <v>12547293</v>
+      </c>
+      <c r="G36">
+        <f>TSIM!G36</f>
+        <v>7121760</v>
+      </c>
+      <c r="H36">
+        <f>TSIM!H36</f>
+        <v>904256</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0394728758010476E-7</v>
+      </c>
+      <c r="K36" s="4">
+        <f t="shared" si="1"/>
+        <v>6.2027802493159481</v>
+      </c>
+      <c r="L36" s="4">
+        <f t="shared" si="2"/>
+        <v>58215184</v>
+      </c>
+      <c r="M36" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6396612113593916</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="3" t="str">
+        <f>TSIM!A37</f>
+        <v>hanoi.O0</v>
+      </c>
+      <c r="B37" s="18">
+        <v>152230657</v>
+      </c>
+      <c r="C37" s="5">
+        <f t="shared" si="4"/>
+        <v>32210181</v>
+      </c>
+      <c r="D37">
+        <v>32210161</v>
+      </c>
+      <c r="E37" s="18">
+        <v>27700110</v>
+      </c>
+      <c r="F37">
+        <f>TSIM!F37</f>
+        <v>27700111</v>
+      </c>
+      <c r="G37">
+        <f>TSIM!G37</f>
+        <v>5410012</v>
+      </c>
+      <c r="H37">
+        <f>TSIM!H37</f>
+        <v>3810020</v>
+      </c>
+      <c r="I37"/>
+      <c r="J37" s="6">
+        <f t="shared" si="0"/>
+        <v>6.2092207486947983E-7</v>
+      </c>
+      <c r="K37" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4956697644882997</v>
+      </c>
+      <c r="L37" s="4">
+        <f t="shared" si="2"/>
+        <v>120020496</v>
+      </c>
+      <c r="M37" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3328526854225489</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="3" t="str">
+        <f>TSIM!A38</f>
+        <v>hanoi.O1</v>
+      </c>
+      <c r="B38" s="18">
+        <v>79055631</v>
+      </c>
+      <c r="C38" s="5">
+        <f t="shared" si="4"/>
+        <v>16965175</v>
+      </c>
+      <c r="D38">
+        <v>16965154</v>
+      </c>
+      <c r="E38" s="18">
+        <v>14805106</v>
+      </c>
+      <c r="F38">
+        <f>TSIM!F38</f>
+        <v>14805107</v>
+      </c>
+      <c r="G38">
+        <f>TSIM!G38</f>
+        <v>1410011</v>
+      </c>
+      <c r="H38">
+        <f>TSIM!H38</f>
+        <v>1460017</v>
+      </c>
+      <c r="I38"/>
+      <c r="J38" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2378313807230986E-6</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3397544738956952</v>
+      </c>
+      <c r="L38" s="4">
+        <f t="shared" si="2"/>
+        <v>62090477</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1938556198111652</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="3" t="str">
+        <f>TSIM!A39</f>
+        <v>hanoi.O2</v>
+      </c>
+      <c r="B39" s="18">
+        <v>69625630</v>
+      </c>
+      <c r="C39" s="5">
+        <f t="shared" si="4"/>
+        <v>14895174</v>
+      </c>
+      <c r="D39">
+        <v>14895154</v>
+      </c>
+      <c r="E39" s="18">
+        <v>12965106</v>
+      </c>
+      <c r="F39">
+        <f>TSIM!F39</f>
+        <v>12965107</v>
+      </c>
+      <c r="G39">
+        <f>TSIM!G39</f>
+        <v>1410011</v>
+      </c>
+      <c r="H39">
+        <f>TSIM!H39</f>
+        <v>1460017</v>
+      </c>
+      <c r="I39"/>
+      <c r="J39" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3427185781362181E-6</v>
+      </c>
+      <c r="K39" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3702322217805234</v>
+      </c>
+      <c r="L39" s="4">
+        <f t="shared" si="2"/>
+        <v>54730476</v>
+      </c>
+      <c r="M39" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2213674149675287</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="3" t="str">
+        <f>TSIM!A40</f>
+        <v>hanoi.O3</v>
+      </c>
+      <c r="B40" s="9">
+        <v>69625630</v>
+      </c>
+      <c r="C40" s="5">
+        <f t="shared" si="4"/>
+        <v>14895174</v>
+      </c>
+      <c r="D40" s="9">
+        <v>14895154</v>
+      </c>
+      <c r="E40" s="9">
+        <v>12965106</v>
+      </c>
+      <c r="F40" s="9">
+        <f>TSIM!F40</f>
+        <v>12965107</v>
+      </c>
+      <c r="G40" s="9">
+        <f>TSIM!G40</f>
+        <v>1410011</v>
+      </c>
+      <c r="H40" s="9">
+        <f>TSIM!H40</f>
+        <v>1460017</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3427185781362181E-6</v>
+      </c>
+      <c r="K40" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3702322217805234</v>
+      </c>
+      <c r="L40" s="4">
+        <f t="shared" si="2"/>
+        <v>54730476</v>
+      </c>
+      <c r="M40" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2213674149675287</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O40" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="3" t="str">
+        <f>TSIM!A41</f>
+        <v>heapsort.O0</v>
+      </c>
+      <c r="B41" s="18">
+        <v>351621292</v>
+      </c>
+      <c r="C41" s="5">
+        <f t="shared" si="4"/>
+        <v>78976906</v>
+      </c>
+      <c r="D41">
+        <v>78976910</v>
+      </c>
+      <c r="E41">
+        <v>64401241</v>
+      </c>
+      <c r="F41">
+        <f>TSIM!F41</f>
+        <v>64401242</v>
+      </c>
+      <c r="G41">
+        <f>TSIM!G41</f>
+        <v>10314820</v>
+      </c>
+      <c r="H41">
+        <f>TSIM!H41</f>
+        <v>4724598</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" si="0"/>
+        <v>5.0647714629503735E-8</v>
+      </c>
+      <c r="K41" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4598527379309356</v>
+      </c>
+      <c r="L41" s="4">
+        <f t="shared" si="2"/>
+        <v>272644382</v>
+      </c>
+      <c r="M41" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2335268352980959</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="3" t="str">
+        <f>TSIM!A42</f>
+        <v>heapsort.O1</v>
+      </c>
+      <c r="B42">
+        <v>187783371</v>
+      </c>
+      <c r="C42" s="5">
+        <f t="shared" si="4"/>
+        <v>46925068</v>
+      </c>
+      <c r="D42">
+        <v>45287951</v>
+      </c>
+      <c r="E42">
+        <v>33828281</v>
+      </c>
+      <c r="F42">
+        <f>TSIM!F42</f>
+        <v>33828282</v>
+      </c>
+      <c r="G42">
+        <f>TSIM!G42</f>
+        <v>3936576</v>
+      </c>
+      <c r="H42">
+        <f>TSIM!H42</f>
+        <v>1608599</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" si="0"/>
+        <v>3.614906313602044E-2</v>
+      </c>
+      <c r="K42" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5510763612256859</v>
+      </c>
+      <c r="L42" s="4">
+        <f t="shared" si="2"/>
+        <v>142495420</v>
+      </c>
+      <c r="M42" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2123163160433723</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="3" t="str">
+        <f>TSIM!A43</f>
+        <v>heapsort.O2</v>
+      </c>
+      <c r="B43">
+        <v>169848370</v>
+      </c>
+      <c r="C43" s="5">
+        <f t="shared" si="4"/>
+        <v>42749511</v>
+      </c>
+      <c r="D43">
+        <v>42149450</v>
+      </c>
+      <c r="E43">
+        <v>30689780</v>
+      </c>
+      <c r="F43">
+        <f>TSIM!F43</f>
+        <v>30689781</v>
+      </c>
+      <c r="G43">
+        <f>TSIM!G43</f>
+        <v>2731136</v>
+      </c>
+      <c r="H43">
+        <f>TSIM!H43</f>
+        <v>1608599</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4236508424190589E-2</v>
+      </c>
+      <c r="K43" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5343625793342275</v>
+      </c>
+      <c r="L43" s="4">
+        <f t="shared" si="2"/>
+        <v>127698920</v>
+      </c>
+      <c r="M43" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1609591205932395</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="3" t="str">
+        <f>TSIM!A44</f>
+        <v>heapsort.O3</v>
+      </c>
+      <c r="B44" s="9">
+        <v>169848370</v>
+      </c>
+      <c r="C44" s="5">
+        <f t="shared" si="4"/>
+        <v>42749511</v>
+      </c>
+      <c r="D44" s="9">
+        <v>42149450</v>
+      </c>
+      <c r="E44" s="9">
+        <v>30689780</v>
+      </c>
+      <c r="F44" s="9">
+        <f>TSIM!F44</f>
+        <v>30689781</v>
+      </c>
+      <c r="G44" s="9">
+        <f>TSIM!G44</f>
+        <v>2731136</v>
+      </c>
+      <c r="H44" s="9">
+        <f>TSIM!H44</f>
+        <v>1608599</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4236508424190589E-2</v>
+      </c>
+      <c r="K44" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5343625793342275</v>
+      </c>
+      <c r="L44" s="4">
+        <f t="shared" si="2"/>
+        <v>127698920</v>
+      </c>
+      <c r="M44" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1609591205932395</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O44" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="3" t="str">
+        <f>TSIM!A45</f>
+        <v>matrix.O0</v>
+      </c>
+      <c r="B45">
+        <v>476722221</v>
+      </c>
+      <c r="C45" s="5">
+        <f t="shared" si="4"/>
+        <v>104268129</v>
+      </c>
+      <c r="D45">
+        <v>104268133</v>
+      </c>
+      <c r="E45">
+        <v>80192666</v>
+      </c>
+      <c r="F45">
+        <f>TSIM!F45</f>
+        <v>80192667</v>
+      </c>
+      <c r="G45">
+        <f>TSIM!G45</f>
+        <v>37800457</v>
+      </c>
+      <c r="H45">
+        <f>TSIM!H45</f>
+        <v>13882967</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8362631850327656E-8</v>
+      </c>
+      <c r="K45" s="4">
+        <f t="shared" si="1"/>
+        <v>5.9447109664616962</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="2"/>
+        <v>372454088</v>
+      </c>
+      <c r="M45" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6444906570383884</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="3" t="str">
+        <f>TSIM!A46</f>
+        <v>matrix.O1</v>
+      </c>
+      <c r="B46">
+        <v>138966313</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" si="4"/>
+        <v>34651264</v>
+      </c>
+      <c r="D46">
+        <v>34651262</v>
+      </c>
+      <c r="E46">
+        <v>24346261</v>
+      </c>
+      <c r="F46">
+        <f>TSIM!F46</f>
+        <v>24346262</v>
+      </c>
+      <c r="G46">
+        <f>TSIM!G46</f>
+        <v>6750000</v>
+      </c>
+      <c r="H46">
+        <f>TSIM!H46</f>
+        <v>180001</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="0"/>
+        <v>5.771795555382658E-8</v>
+      </c>
+      <c r="K46" s="4">
+        <f t="shared" si="1"/>
+        <v>5.7079119048300679</v>
+      </c>
+      <c r="L46" s="4">
+        <f t="shared" si="2"/>
+        <v>104315051</v>
+      </c>
+      <c r="M46" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2846435844912696</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="3" t="str">
+        <f>TSIM!A47</f>
+        <v>matrix.O2</v>
+      </c>
+      <c r="B47">
+        <v>162432278</v>
+      </c>
+      <c r="C47" s="5">
+        <f t="shared" si="4"/>
+        <v>41355957</v>
+      </c>
+      <c r="D47">
+        <v>41355955</v>
+      </c>
+      <c r="E47">
+        <v>27698454</v>
+      </c>
+      <c r="F47">
+        <f>TSIM!F47</f>
+        <v>27698455</v>
+      </c>
+      <c r="G47">
+        <f>TSIM!G47</f>
+        <v>6750000</v>
+      </c>
+      <c r="H47">
+        <f>TSIM!H47</f>
+        <v>3532501</v>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8360629079899132E-8</v>
+      </c>
+      <c r="K47" s="4">
+        <f t="shared" si="1"/>
+        <v>5.8643084556271621</v>
+      </c>
+      <c r="L47" s="4">
+        <f t="shared" si="2"/>
+        <v>121076323</v>
+      </c>
+      <c r="M47" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3712303581997753</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="3" t="str">
+        <f>TSIM!A48</f>
+        <v>matrix.O3</v>
+      </c>
+      <c r="B48" s="9">
+        <v>162432278</v>
+      </c>
+      <c r="C48" s="5">
+        <f t="shared" si="4"/>
+        <v>41355957</v>
+      </c>
+      <c r="D48" s="9">
+        <v>41355955</v>
+      </c>
+      <c r="E48" s="9">
+        <v>27698454</v>
+      </c>
+      <c r="F48" s="9">
+        <f>TSIM!F48</f>
+        <v>27698455</v>
+      </c>
+      <c r="G48" s="9">
+        <f>TSIM!G48</f>
+        <v>6750000</v>
+      </c>
+      <c r="H48" s="9">
+        <f>TSIM!H48</f>
+        <v>3532501</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8360629079899132E-8</v>
+      </c>
+      <c r="K48" s="4">
+        <f t="shared" si="1"/>
+        <v>5.8643084556271621</v>
+      </c>
+      <c r="L48" s="4">
+        <f t="shared" si="2"/>
+        <v>121076323</v>
+      </c>
+      <c r="M48" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3712303581997753</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O48" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="3" t="str">
+        <f>TSIM!A49</f>
+        <v>pocsag.O0</v>
+      </c>
+      <c r="B49">
+        <v>57167605</v>
+      </c>
+      <c r="C49" s="5">
+        <f t="shared" si="4"/>
+        <v>11690317</v>
+      </c>
+      <c r="D49">
+        <v>11690321</v>
+      </c>
+      <c r="E49">
+        <v>10493620</v>
+      </c>
+      <c r="F49">
+        <f>TSIM!F49</f>
+        <v>10493621</v>
+      </c>
+      <c r="G49">
+        <f>TSIM!G49</f>
+        <v>2360601</v>
+      </c>
+      <c r="H49">
+        <f>TSIM!H49</f>
+        <v>1142203</v>
+      </c>
+      <c r="J49" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4216340167220385E-7</v>
+      </c>
+      <c r="K49" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4478440233208367</v>
+      </c>
+      <c r="L49" s="4">
+        <f t="shared" si="2"/>
+        <v>45477284</v>
+      </c>
+      <c r="M49" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3338032061385867</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="3" t="str">
+        <f>TSIM!A50</f>
+        <v>pocsag.O1</v>
+      </c>
+      <c r="B50">
+        <v>17888985</v>
+      </c>
+      <c r="C50" s="5">
+        <f t="shared" si="4"/>
+        <v>3670212</v>
+      </c>
+      <c r="D50">
+        <v>3554716</v>
+      </c>
+      <c r="E50">
+        <v>3450017</v>
+      </c>
+      <c r="F50">
+        <f>TSIM!F50</f>
+        <v>3450018</v>
+      </c>
+      <c r="G50">
+        <f>TSIM!G50</f>
+        <v>368500</v>
+      </c>
+      <c r="H50">
+        <f>TSIM!H50</f>
+        <v>50201</v>
+      </c>
+      <c r="J50" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2490921918938112E-2</v>
+      </c>
+      <c r="K50" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1851874932790185</v>
+      </c>
+      <c r="L50" s="4">
+        <f t="shared" si="2"/>
+        <v>14334269</v>
+      </c>
+      <c r="M50" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1548401065849818</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="3" t="str">
+        <f>TSIM!A51</f>
+        <v>pocsag.O2</v>
+      </c>
+      <c r="B51">
+        <v>15259991</v>
+      </c>
+      <c r="C51" s="5">
+        <f t="shared" si="4"/>
+        <v>3125814</v>
+      </c>
+      <c r="D51">
+        <v>3034217</v>
+      </c>
+      <c r="E51">
+        <v>2929518</v>
+      </c>
+      <c r="F51">
+        <f>TSIM!F51</f>
+        <v>2929519</v>
+      </c>
+      <c r="G51">
+        <f>TSIM!G51</f>
+        <v>365900</v>
+      </c>
+      <c r="H51">
+        <f>TSIM!H51</f>
+        <v>50201</v>
+      </c>
+      <c r="J51" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0188018852969317E-2</v>
+      </c>
+      <c r="K51" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2090449691724032</v>
+      </c>
+      <c r="L51" s="4">
+        <f t="shared" si="2"/>
+        <v>12225774</v>
+      </c>
+      <c r="M51" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1733056427712683</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="3" t="str">
+        <f>TSIM!A52</f>
+        <v>pocsag.O3</v>
+      </c>
+      <c r="B52">
+        <v>14831591</v>
+      </c>
+      <c r="C52" s="5">
+        <f t="shared" si="4"/>
+        <v>3040214</v>
+      </c>
+      <c r="D52">
+        <v>2948517</v>
+      </c>
+      <c r="E52">
+        <v>2843818</v>
+      </c>
+      <c r="F52">
+        <f>TSIM!F52</f>
+        <v>2843819</v>
+      </c>
+      <c r="G52">
+        <f>TSIM!G52</f>
+        <v>365900</v>
+      </c>
+      <c r="H52">
+        <f>TSIM!H52</f>
+        <v>50201</v>
+      </c>
+      <c r="J52" s="6">
+        <f t="shared" si="0"/>
+        <v>3.1099362832230575E-2</v>
+      </c>
+      <c r="K52" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2153798168518524</v>
+      </c>
+      <c r="L52" s="4">
+        <f t="shared" si="2"/>
+        <v>11883074</v>
+      </c>
+      <c r="M52" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1785634664384288</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="3" t="str">
+        <f>TSIM!A53</f>
+        <v>queens.O0</v>
+      </c>
+      <c r="B53">
+        <v>40147242</v>
+      </c>
+      <c r="C53" s="5">
+        <f t="shared" si="4"/>
+        <v>8022576</v>
+      </c>
+      <c r="D53">
+        <v>7998964</v>
+      </c>
+      <c r="E53">
+        <v>7684292</v>
+      </c>
+      <c r="F53">
+        <f>TSIM!F53</f>
+        <v>7684293</v>
+      </c>
+      <c r="G53">
+        <f>TSIM!G53</f>
+        <v>1130018</v>
+      </c>
+      <c r="H53">
+        <f>TSIM!H53</f>
+        <v>257476</v>
+      </c>
+      <c r="I53"/>
+      <c r="J53" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9518822687538038E-3</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2245856872695624</v>
+      </c>
+      <c r="L53" s="4">
+        <f t="shared" si="2"/>
+        <v>32148278</v>
+      </c>
+      <c r="M53" s="4">
+        <f t="shared" si="3"/>
+        <v>4.183635655698664</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="3" t="str">
+        <f>TSIM!A54</f>
+        <v>queens.O1</v>
+      </c>
+      <c r="B54">
+        <v>28966547</v>
+      </c>
+      <c r="C54" s="5">
+        <f t="shared" si="4"/>
+        <v>5990323</v>
+      </c>
+      <c r="D54">
+        <v>5756104</v>
+      </c>
+      <c r="E54">
+        <v>5441434</v>
+      </c>
+      <c r="F54">
+        <f>TSIM!F54</f>
+        <v>5441435</v>
+      </c>
+      <c r="G54">
+        <f>TSIM!G54</f>
+        <v>953010</v>
+      </c>
+      <c r="H54">
+        <f>TSIM!H54</f>
+        <v>257474</v>
+      </c>
+      <c r="I54"/>
+      <c r="J54" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0690543464815786E-2</v>
+      </c>
+      <c r="K54" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3233296590567853</v>
+      </c>
+      <c r="L54" s="4">
+        <f t="shared" si="2"/>
+        <v>23210443</v>
+      </c>
+      <c r="M54" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2655011528211126</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="3" t="str">
+        <f>TSIM!A55</f>
+        <v>queens.O2</v>
+      </c>
+      <c r="B55">
+        <v>27567934</v>
+      </c>
+      <c r="C55" s="5">
+        <f t="shared" si="4"/>
+        <v>5705790</v>
+      </c>
+      <c r="D55">
+        <v>5477584</v>
+      </c>
+      <c r="E55">
+        <v>5162914</v>
+      </c>
+      <c r="F55">
+        <f>TSIM!F55</f>
+        <v>5162915</v>
+      </c>
+      <c r="G55">
+        <f>TSIM!G55</f>
+        <v>953010</v>
+      </c>
+      <c r="H55">
+        <f>TSIM!H55</f>
+        <v>257474</v>
+      </c>
+      <c r="I55"/>
+      <c r="J55" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1661798340290171E-2</v>
+      </c>
+      <c r="K55" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3396074387448635</v>
+      </c>
+      <c r="L55" s="4">
+        <f t="shared" si="2"/>
+        <v>22090350</v>
+      </c>
+      <c r="M55" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2786592997675346</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="3" t="str">
+        <f>TSIM!A56</f>
+        <v>queens.O3</v>
+      </c>
+      <c r="B56" s="4">
+        <v>27531658</v>
+      </c>
+      <c r="C56" s="5">
+        <f t="shared" si="4"/>
+        <v>5746164</v>
+      </c>
+      <c r="D56">
+        <v>5517958</v>
+      </c>
+      <c r="E56" s="4">
+        <v>5203288</v>
+      </c>
+      <c r="F56">
+        <f>TSIM!F56</f>
+        <v>5203289</v>
+      </c>
+      <c r="G56">
+        <f>TSIM!G56</f>
+        <v>714864</v>
+      </c>
+      <c r="H56">
+        <f>TSIM!H56</f>
+        <v>257474</v>
+      </c>
+      <c r="J56" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1356965747111521E-2</v>
+      </c>
+      <c r="K56" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2912039464277205</v>
+      </c>
+      <c r="L56" s="4">
+        <f t="shared" si="2"/>
+        <v>22013700</v>
+      </c>
+      <c r="M56" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2307287238376965</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="3" t="str">
+        <f>TSIM!A57</f>
+        <v>quicksort.O0</v>
+      </c>
+      <c r="B57">
+        <v>86436606</v>
+      </c>
+      <c r="C57" s="5">
+        <f t="shared" si="4"/>
+        <v>17494498</v>
+      </c>
+      <c r="D57">
+        <v>17422913</v>
+      </c>
+      <c r="E57">
+        <v>15536052</v>
+      </c>
+      <c r="F57">
+        <f>TSIM!F57</f>
+        <v>15536052</v>
+      </c>
+      <c r="G57">
+        <f>TSIM!G57</f>
+        <v>5244269</v>
+      </c>
+      <c r="H57">
+        <f>TSIM!H57</f>
+        <v>1553631</v>
+      </c>
+      <c r="I57"/>
+      <c r="J57" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1086700025420551E-3</v>
+      </c>
+      <c r="K57" s="4">
+        <f t="shared" si="1"/>
+        <v>5.56361461714984</v>
+      </c>
+      <c r="L57" s="4">
+        <f t="shared" si="2"/>
+        <v>69013693</v>
+      </c>
+      <c r="M57" s="4">
+        <f t="shared" si="3"/>
+        <v>4.4421641353929555</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="3" t="str">
+        <f>TSIM!A58</f>
+        <v>quicksort.O1</v>
+      </c>
+      <c r="B58">
+        <v>40234047</v>
+      </c>
+      <c r="C58" s="5">
+        <f t="shared" si="4"/>
+        <v>8517767</v>
+      </c>
+      <c r="D58">
+        <v>8306373</v>
+      </c>
+      <c r="E58">
+        <v>7597840</v>
+      </c>
+      <c r="F58">
+        <f>TSIM!F58</f>
+        <v>7597840</v>
+      </c>
+      <c r="G58">
+        <f>TSIM!G58</f>
+        <v>949617</v>
+      </c>
+      <c r="H58">
+        <f>TSIM!H58</f>
+        <v>375303</v>
+      </c>
+      <c r="I58"/>
+      <c r="J58" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5449615614420398E-2</v>
+      </c>
+      <c r="K58" s="4">
+        <f t="shared" si="1"/>
+        <v>5.295458577701031</v>
+      </c>
+      <c r="L58" s="4">
+        <f t="shared" si="2"/>
+        <v>31927674</v>
+      </c>
+      <c r="M58" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2022040474661218</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="3" t="str">
+        <f>TSIM!A59</f>
+        <v>quicksort.O2</v>
+      </c>
+      <c r="B59">
+        <v>38194800</v>
+      </c>
+      <c r="C59" s="5">
+        <f t="shared" si="4"/>
+        <v>7917674</v>
+      </c>
+      <c r="D59">
+        <v>7887237</v>
+      </c>
+      <c r="E59">
+        <v>7246561</v>
+      </c>
+      <c r="F59">
+        <f>TSIM!F59</f>
+        <v>7246561</v>
+      </c>
+      <c r="G59">
+        <f>TSIM!G59</f>
+        <v>930707</v>
+      </c>
+      <c r="H59">
+        <f>TSIM!H59</f>
+        <v>360175</v>
+      </c>
+      <c r="I59"/>
+      <c r="J59" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8590193245112325E-3</v>
+      </c>
+      <c r="K59" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2707484281164545</v>
+      </c>
+      <c r="L59" s="4">
+        <f t="shared" si="2"/>
+        <v>30307563</v>
+      </c>
+      <c r="M59" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1823373873482881</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="3" t="str">
+        <f>TSIM!A60</f>
+        <v>quicksort.O3</v>
+      </c>
+      <c r="B60" s="9">
+        <v>38194800</v>
+      </c>
+      <c r="C60" s="5">
+        <f t="shared" si="4"/>
+        <v>7917674</v>
+      </c>
+      <c r="D60" s="9">
+        <v>7887237</v>
+      </c>
+      <c r="E60" s="9">
+        <v>7246561</v>
+      </c>
+      <c r="F60" s="9">
+        <f>TSIM!F60</f>
+        <v>7246561</v>
+      </c>
+      <c r="G60" s="9">
+        <f>TSIM!G60</f>
+        <v>930707</v>
+      </c>
+      <c r="H60" s="9">
+        <f>TSIM!H60</f>
+        <v>360175</v>
+      </c>
+      <c r="I60" s="9"/>
+      <c r="J60" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8590193245112325E-3</v>
+      </c>
+      <c r="K60" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2707484281164545</v>
+      </c>
+      <c r="L60" s="4">
+        <f t="shared" si="2"/>
+        <v>30307563</v>
+      </c>
+      <c r="M60" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1823373873482881</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O60" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15" customHeight="1">
+      <c r="C63" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+    </row>
+    <row r="65" spans="3:11">
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="22"/>
+    </row>
+    <row r="66" spans="3:11">
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+    </row>
+    <row r="67" spans="3:11">
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+    </row>
+    <row r="68" spans="3:11">
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+    </row>
+    <row r="69" spans="3:11">
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+      <c r="K69" s="22"/>
+    </row>
+    <row r="70" spans="3:11">
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="22"/>
+      <c r="K70" s="22"/>
+    </row>
+    <row r="71" spans="3:11">
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="22"/>
+      <c r="K71" s="22"/>
+    </row>
+    <row r="72" spans="3:11">
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="22"/>
+    </row>
+    <row r="73" spans="3:11">
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+    </row>
+    <row r="74" spans="3:11">
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="22"/>
+    </row>
+    <row r="75" spans="3:11">
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+    </row>
+    <row r="76" spans="3:11">
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="22"/>
+    </row>
+    <row r="77" spans="3:11">
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="22"/>
+    </row>
+    <row r="78" spans="3:11">
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="22"/>
+    </row>
+    <row r="79" spans="3:11">
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="22"/>
+    </row>
+    <row r="80" spans="3:11">
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="22"/>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" s="3" t="str">
+        <f>TSIM!A82</f>
+        <v>just nops</v>
+      </c>
+      <c r="B82">
+        <v>49800124</v>
+      </c>
+      <c r="C82" s="5">
+        <f t="shared" ref="C82:C91" si="6">B82-($C$2*F82+G82*$D$2+H82*$E$2)</f>
+        <v>9960025</v>
+      </c>
+      <c r="D82">
+        <f>TSIM!D82</f>
+        <v>9960029</v>
+      </c>
+      <c r="E82">
+        <v>9960024</v>
+      </c>
+      <c r="F82">
+        <f>TSIM!F82</f>
+        <v>9960024</v>
+      </c>
+      <c r="G82">
+        <f>TSIM!G82</f>
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <f>TSIM!H82</f>
+        <v>3</v>
+      </c>
+      <c r="I82"/>
+      <c r="J82" s="6">
+        <f t="shared" ref="J82:J91" si="7">IF(D82 = 0, "", ABS(C82-D82)/D82)</f>
+        <v>4.0160525637023747E-7</v>
+      </c>
+      <c r="K82" s="4">
+        <f t="shared" ref="K82:K91" si="8">B82/E82</f>
+        <v>5.0000004016054582</v>
+      </c>
+      <c r="L82" s="4">
+        <f t="shared" ref="L82:L91" si="9">B82-D82</f>
+        <v>39840095</v>
+      </c>
+      <c r="M82" s="4">
+        <f t="shared" ref="M82:M91" si="10">L82/E82</f>
+        <v>3.9999998995986354</v>
+      </c>
+      <c r="N82">
+        <f t="shared" ref="N82:N91" si="11">E82-F82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" s="3" t="str">
+        <f>TSIM!A83</f>
+        <v>increment_var</v>
+      </c>
+      <c r="B83">
+        <v>178500124</v>
+      </c>
+      <c r="C83" s="5">
+        <f t="shared" si="6"/>
+        <v>39660025</v>
+      </c>
+      <c r="D83">
+        <f>TSIM!D83</f>
+        <v>39660029</v>
+      </c>
+      <c r="E83">
+        <v>29760024</v>
+      </c>
+      <c r="F83">
+        <f>TSIM!F83</f>
+        <v>29760024</v>
+      </c>
+      <c r="G83">
+        <f>TSIM!G83</f>
+        <v>9900000</v>
+      </c>
+      <c r="H83">
+        <f>TSIM!H83</f>
+        <v>9900003</v>
+      </c>
+      <c r="I83"/>
+      <c r="J83" s="6">
+        <f t="shared" si="7"/>
+        <v>1.0085721319064088E-7</v>
+      </c>
+      <c r="K83" s="4">
+        <f t="shared" si="8"/>
+        <v>5.9979832005511824</v>
+      </c>
+      <c r="L83" s="4">
+        <f t="shared" si="9"/>
+        <v>138840095</v>
+      </c>
+      <c r="M83" s="4">
+        <f t="shared" si="10"/>
+        <v>4.6653220104930027</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" s="3" t="str">
+        <f>TSIM!A84</f>
+        <v>increment_reg</v>
+      </c>
+      <c r="B84">
+        <v>49800124</v>
+      </c>
+      <c r="C84" s="5">
+        <f t="shared" si="6"/>
+        <v>9960021</v>
+      </c>
+      <c r="D84">
+        <f>TSIM!D84</f>
+        <v>9960030</v>
+      </c>
+      <c r="E84">
+        <v>9960025</v>
+      </c>
+      <c r="F84">
+        <f>TSIM!F84</f>
+        <v>9960025</v>
+      </c>
+      <c r="G84">
+        <f>TSIM!G84</f>
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <f>TSIM!H84</f>
+        <v>3</v>
+      </c>
+      <c r="I84"/>
+      <c r="J84" s="6">
+        <f t="shared" si="7"/>
+        <v>9.0361173610922863E-7</v>
+      </c>
+      <c r="K84" s="4">
+        <f t="shared" si="8"/>
+        <v>4.9999998995986452</v>
+      </c>
+      <c r="L84" s="4">
+        <f t="shared" si="9"/>
+        <v>39840094</v>
+      </c>
+      <c r="M84" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9999993975918735</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
+      <c r="A85" s="3" t="str">
+        <f>TSIM!A85</f>
+        <v>just_load</v>
+      </c>
+      <c r="B85">
+        <v>59700119</v>
+      </c>
+      <c r="C85" s="5">
+        <f t="shared" si="6"/>
+        <v>9960020</v>
+      </c>
+      <c r="D85">
+        <f>TSIM!D85</f>
+        <v>9960029</v>
+      </c>
+      <c r="E85">
+        <v>9960023</v>
+      </c>
+      <c r="F85">
+        <f>TSIM!F85</f>
+        <v>9960024</v>
+      </c>
+      <c r="G85">
+        <f>TSIM!G85</f>
+        <v>9900000</v>
+      </c>
+      <c r="H85">
+        <f>TSIM!H85</f>
+        <v>3</v>
+      </c>
+      <c r="I85"/>
+      <c r="J85" s="6">
+        <f t="shared" si="7"/>
+        <v>9.0361182683303428E-7</v>
+      </c>
+      <c r="K85" s="4">
+        <f t="shared" si="8"/>
+        <v>5.9939740098993743</v>
+      </c>
+      <c r="L85" s="4">
+        <f t="shared" si="9"/>
+        <v>49740090</v>
+      </c>
+      <c r="M85" s="4">
+        <f t="shared" si="10"/>
+        <v>4.9939734074911275</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
+      <c r="A86" s="3" t="str">
+        <f>TSIM!A86</f>
+        <v>just_store</v>
+      </c>
+      <c r="B86">
+        <v>69600119</v>
+      </c>
+      <c r="C86" s="5">
+        <f t="shared" si="6"/>
+        <v>19860020</v>
+      </c>
+      <c r="D86">
+        <f>TSIM!D86</f>
+        <v>19860029</v>
+      </c>
+      <c r="E86">
+        <v>9960023</v>
+      </c>
+      <c r="F86">
+        <f>TSIM!F86</f>
+        <v>9960024</v>
+      </c>
+      <c r="G86">
+        <f>TSIM!G86</f>
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <f>TSIM!H86</f>
+        <v>9900003</v>
+      </c>
+      <c r="I86"/>
+      <c r="J86" s="6">
+        <f t="shared" si="7"/>
+        <v>4.5317154370721212E-7</v>
+      </c>
+      <c r="K86" s="4">
+        <f t="shared" si="8"/>
+        <v>6.9879476181932514</v>
+      </c>
+      <c r="L86" s="4">
+        <f t="shared" si="9"/>
+        <v>49740090</v>
+      </c>
+      <c r="M86" s="4">
+        <f t="shared" si="10"/>
+        <v>4.9939734074911275</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" s="3" t="str">
+        <f>TSIM!A87</f>
+        <v>sum vars</v>
+      </c>
+      <c r="B87">
+        <v>237900126</v>
+      </c>
+      <c r="C87" s="5">
+        <f t="shared" si="6"/>
+        <v>49560027</v>
+      </c>
+      <c r="D87">
+        <f>TSIM!D87</f>
+        <v>49560029</v>
+      </c>
+      <c r="E87">
+        <v>39660024</v>
+      </c>
+      <c r="F87">
+        <f>TSIM!F87</f>
+        <v>39660024</v>
+      </c>
+      <c r="G87">
+        <f>TSIM!G87</f>
+        <v>19800000</v>
+      </c>
+      <c r="H87">
+        <f>TSIM!H87</f>
+        <v>9900003</v>
+      </c>
+      <c r="I87"/>
+      <c r="J87" s="6">
+        <f t="shared" si="7"/>
+        <v>4.0355101487127863E-8</v>
+      </c>
+      <c r="K87" s="4">
+        <f t="shared" si="8"/>
+        <v>5.9984866877538954</v>
+      </c>
+      <c r="L87" s="4">
+        <f t="shared" si="9"/>
+        <v>188340097</v>
+      </c>
+      <c r="M87" s="4">
+        <f t="shared" si="10"/>
+        <v>4.7488649275653492</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88">
+        <v>129000124</v>
+      </c>
+      <c r="C88" s="5">
+        <f t="shared" si="6"/>
+        <v>49560021</v>
+      </c>
+      <c r="D88">
+        <v>49560029</v>
+      </c>
+      <c r="E88">
+        <v>19860024</v>
+      </c>
+      <c r="F88">
+        <v>19860025</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>3</v>
+      </c>
+      <c r="J88" s="6">
+        <f t="shared" si="7"/>
+        <v>1.6142040594851145E-7</v>
+      </c>
+      <c r="K88" s="4">
+        <f t="shared" si="8"/>
+        <v>6.4954666721450085</v>
+      </c>
+      <c r="L88" s="4">
+        <f t="shared" si="9"/>
+        <v>79440095</v>
+      </c>
+      <c r="M88" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9999999496475938</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="O88" s="20"/>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>683400124</v>
+      </c>
+      <c r="C89" s="5">
+        <f t="shared" si="6"/>
+        <v>405960021</v>
+      </c>
+      <c r="D89">
+        <v>405960029</v>
+      </c>
+      <c r="E89">
+        <v>69360024</v>
+      </c>
+      <c r="F89">
+        <v>69360025</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>3</v>
+      </c>
+      <c r="J89" s="6">
+        <f t="shared" si="7"/>
+        <v>1.9706373604579677E-8</v>
+      </c>
+      <c r="K89" s="4">
+        <f t="shared" si="8"/>
+        <v>9.8529395549228767</v>
+      </c>
+      <c r="L89" s="4">
+        <f t="shared" si="9"/>
+        <v>277440095</v>
+      </c>
+      <c r="M89" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9999999855824733</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="O89" s="20"/>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90">
+        <v>505200124</v>
+      </c>
+      <c r="C90" s="5">
+        <f t="shared" si="6"/>
+        <v>108960021</v>
+      </c>
+      <c r="D90">
+        <v>108960029</v>
+      </c>
+      <c r="E90">
+        <v>99060024</v>
+      </c>
+      <c r="F90">
+        <v>99060025</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>3</v>
+      </c>
+      <c r="J90" s="6">
+        <f t="shared" si="7"/>
+        <v>7.3421419518895312E-8</v>
+      </c>
+      <c r="K90" s="4">
+        <f t="shared" si="8"/>
+        <v>5.0999394468145898</v>
+      </c>
+      <c r="L90" s="4">
+        <f t="shared" si="9"/>
+        <v>396240095</v>
+      </c>
+      <c r="M90" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9999999899051106</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="O90" s="20"/>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="A91" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91">
+        <v>79500124</v>
+      </c>
+      <c r="C91" s="5">
+        <f t="shared" si="6"/>
+        <v>39660005</v>
+      </c>
+      <c r="D91">
+        <v>39660029</v>
+      </c>
+      <c r="E91">
+        <v>9960024</v>
+      </c>
+      <c r="F91">
+        <v>9960029</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>3</v>
+      </c>
+      <c r="J91" s="6">
+        <f t="shared" si="7"/>
+        <v>6.0514327914384527E-7</v>
+      </c>
+      <c r="K91" s="4">
+        <f t="shared" si="8"/>
+        <v>7.9819209270981677</v>
+      </c>
+      <c r="L91" s="4">
+        <f t="shared" si="9"/>
+        <v>39840095</v>
+      </c>
+      <c r="M91" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9999998995986354</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="11"/>
+        <v>-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A4:O4">
+    <sortState ref="A5:O60">
+      <sortCondition ref="A4"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="5">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="C63:K80"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J5:J60 J82:J91">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C60">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="greaterThan">
+      <formula>D5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="greaterThan">
+      <formula>L2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F60">
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>((ABS($E5-$F5))/$E5) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C88">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
+      <formula>D82</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E82:F82">
+    <cfRule type="expression" dxfId="26" priority="27">
+      <formula>((ABS($E82-$F82))/$E82) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
+      <formula>D83</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83:F83">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>((ABS($E83-$F83))/$E83) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+      <formula>D84</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:F84">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>((ABS($E84-$F84))/$E84) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
+      <formula>D85</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:F85">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>((ABS($E85-$F85))/$E85) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+      <formula>D86</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86:F86">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>((ABS($E86-$F86))/$E86) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E87">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87:C88">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
+      <formula>D87</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E87:F87">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>((ABS($E87-$F87))/$E87) &gt; 0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C88">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+      <formula>D82</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C88">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+      <formula>D82</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
+      <formula>D89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>D89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>D89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+      <formula>D89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>D90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>D90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>D90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>D90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>D91</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>D91</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>D91</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>D91</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>